<commit_message>
Working on db caching, created data layer and db
</commit_message>
<xml_diff>
--- a/Database and update schema.xlsx
+++ b/Database and update schema.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamc\PycharmProjects\continuous-outline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3842BEF-9F1E-48F6-95BC-1BEDC72B92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1579FB5B-B0B8-4679-B12D-327411E40189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="1995" windowWidth="16440" windowHeight="29040" xr2:uid="{AD75AE63-7256-49E8-B3A4-5543BDBDEB26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Focus Mask</t>
   </si>
@@ -72,23 +73,231 @@
     <t>Agent</t>
   </si>
   <si>
-    <t>Path Tracker</t>
-  </si>
-  <si>
     <t>Path Node</t>
+  </si>
+  <si>
+    <t>Raw Path</t>
+  </si>
+  <si>
+    <t>Formed Path</t>
+  </si>
+  <si>
+    <t>StartNode</t>
+  </si>
+  <si>
+    <t>EndNode</t>
+  </si>
+  <si>
+    <t>ContourNum</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Trackers</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>CustomWeight</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>FocusRegionSections</t>
+  </si>
+  <si>
+    <t>Ygrade</t>
+  </si>
+  <si>
+    <t>Xgrade</t>
+  </si>
+  <si>
+    <t>y_sec</t>
+  </si>
+  <si>
+    <t>x_sec</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>focus_region</t>
+  </si>
+  <si>
+    <t>focus_region_nums</t>
+  </si>
+  <si>
+    <t>dumb_req</t>
+  </si>
+  <si>
+    <t>dumb_opt</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Sections (
+  height INTEGER,
+  width INTEGER,
+  focus_region_sections TEXT,
+  sections TEXT,
+  y_grade REAL,
+  x_grade REAL
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE EdgePath (
+  contour_num INTEGER,
+  path TEXT,
+  trackers TEXT,
+  is_outer INTEGER,
+  is_closed INTEGER,
+  custom_weight REAL
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Agent (
+  start_node INTEGER,  end_node INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Section (
+  y_sec INTEGER,
+  x_sec INTEGER,
+  nodes TEXT,
+  focus_region TEXT,
+  focus_region_nums TEXT,
+  dumb_req INTEGER,
+  dumb_opt INTEGER
+);</t>
+  </si>
+  <si>
+    <t>SectionTracker</t>
+  </si>
+  <si>
+    <t>CREATE TABLE SectionTracker (
+  section INTEGER,
+  nodes TEXT,
+  in_node INTEGER,
+  out_node INTEGER,
+  path TEXT,
+  path_num INTEGER,
+  rev_in_node INTEGER,
+  rev_out_node INTEGER,
+  tracker_num INTEGER,
+  prev_tracker INTEGER,
+  next_tracker INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE PathNode (
+  y INTEGER,
+  x INTEGER,
+  path TEXT,
+  section_id INTEGER,
+  section_tracker_id INTEGER,
+  node INTEGER,
+is_outer INTEGER);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE GraphEdge (
+  from_node INTEGER,
+  to_node INTEGER,
+  weight REAL
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE GraphNode (
+  graph_node INTEGER, graph_node_y INTEGER, graph_node_x INTEGER, graph_node_path INTEGER, graph_node_tracker INTEGER,
+  category TEXT
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE RawPath (
+  y INTEGER,
+  x INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE FormedPath (
+  y REAL,
+  x REAL
+);</t>
+  </si>
+  <si>
+    <t>Focus Masks</t>
+  </si>
+  <si>
+    <t>CREATE TABLE FocusMasks (
+  focus_mask INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE FocusMask (focus_mask INTEGER, 
+  y INTEGER,
+  x INTEGER);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE EdgesPixelMap (
+  y INTEGER,
+  x INTEGER,
+  is_inner INTEGER,
+  is_outer INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Contour (
+  contour INTEGER,
+  y INTEGER,
+  x INTEGER
+);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE Contours (
+  contour INTEGER,
+  is_outer INTEGER,
+  is_inner INTEGER
+);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.4"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.4"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +320,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,69 +649,599 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684014D8-7733-408F-A873-ECB07C129634}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2">
         <v>1</v>
       </c>
-      <c r="E1">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2">
+        <v>3</v>
+      </c>
+      <c r="O1" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="409.5">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="50">
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="25">
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="G10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="10:10">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="10:10">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="10:10">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="10:10">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="10:10">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="10:10">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="10:10">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="10:10">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="10:10">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="10:10">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="10:10">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="10:10">
+      <c r="J28" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3A8105-827F-402F-8DB0-53F734AEBAFB}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="159.5">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" ht="159.5">
+      <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="188.5">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" ht="130.5">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" ht="174">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" ht="290">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" ht="377">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" ht="377">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" ht="203">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" ht="159.5">
+      <c r="A10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" ht="319">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" ht="409.5">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" ht="333.5">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" ht="130.5">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" ht="101.5">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>